<commit_message>
contains fresh new modifications, reading excel file and change graph
</commit_message>
<xml_diff>
--- a/inputfile.xlsx
+++ b/inputfile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t xml:space="preserve">&lt;task_name&gt;</t>
   </si>
@@ -34,10 +34,16 @@
     <t xml:space="preserve">&lt;op1&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;op2&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;op3&gt;</t>
+    <t xml:space="preserve">&lt;op12&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;op2-13&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;op1, op12&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;END&gt;</t>
   </si>
 </sst>
 </file>
@@ -52,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -111,9 +118,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -133,25 +148,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -159,30 +176,38 @@
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>